<commit_message>
fixed eval wrong table orientation
</commit_message>
<xml_diff>
--- a/progress_tracking/progress.xlsx
+++ b/progress_tracking/progress.xlsx
@@ -527,7 +527,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>18.11.2025 11:42</t>
+          <t>18.11.2025 13:02</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
@@ -541,13 +541,13 @@
         </is>
       </c>
       <c r="D4" s="3" t="n">
-        <v>122.24413375</v>
+        <v>130.95238746</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>35658.62631007409</v>
+        <v>35628.05096234559</v>
       </c>
       <c r="F4" s="3" t="n">
-        <v>23.905724</v>
+        <v>28.451178</v>
       </c>
     </row>
   </sheetData>
@@ -672,6 +672,26 @@
         <color rgb="00F8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="colorScale" priority="20">
@@ -734,6 +754,26 @@
         <color rgb="00F8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="colorScale" priority="3">
@@ -847,6 +887,26 @@
       </colorScale>
     </cfRule>
     <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00F8696B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="0063BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00F8696B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="0063BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
integrated material eval into psqt
</commit_message>
<xml_diff>
--- a/progress_tracking/progress.xlsx
+++ b/progress_tracking/progress.xlsx
@@ -1,115 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6BEBAD-A123-4962-89AF-596647DD2293}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="3465" windowWidth="24615" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="195" yWindow="3465" windowWidth="24615" windowHeight="11295" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Progress" sheetId="1" r:id="rId1"/>
+    <sheet name="Progress" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>TIMESTAMP</t>
-  </si>
-  <si>
-    <t>COMMIT</t>
-  </si>
-  <si>
-    <t>MESSAGE</t>
-  </si>
-  <si>
-    <t>PERFT (ms)</t>
-  </si>
-  <si>
-    <t>EVAL (ps)</t>
-  </si>
-  <si>
-    <t>SUITE (%)</t>
-  </si>
-  <si>
-    <t>15.11.2025 18:44</t>
-  </si>
-  <si>
-    <t>96ea7fd</t>
-  </si>
-  <si>
-    <t>fixed progress tracking</t>
-  </si>
-  <si>
-    <t>17.11.2025 08:30</t>
-  </si>
-  <si>
-    <t>e62ed41</t>
-  </si>
-  <si>
-    <t>alpha beta pruning</t>
-  </si>
-  <si>
-    <t>18.11.2025 16:27</t>
-  </si>
-  <si>
-    <t>32be42e</t>
-  </si>
-  <si>
-    <t>piece square evaluation</t>
-  </si>
-  <si>
-    <t>0c1055d</t>
-  </si>
-  <si>
-    <t>fixed eval wrong table orientation</t>
-  </si>
-  <si>
-    <t>ecf1de6</t>
-  </si>
-  <si>
-    <t>iterative deepening</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Consolas"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Consolas"/>
     </font>
     <font>
+      <name val="Consolas"/>
       <sz val="11"/>
-      <name val="Consolas"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -128,37 +61,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -446,139 +438,209 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="6" width="14" customWidth="1"/>
+    <col width="20" customWidth="1" style="8" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="6"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>COMMIT</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MESSAGE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PERFT (ms)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EVAL (ps)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SUITE (%)</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3">
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>15.11.2025 18:44</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>96ea7fd</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>fixed progress tracking</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>104.547059</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <v>208.1159881736437</v>
       </c>
-      <c r="F2" s="3">
-        <v>17.676767000000002</v>
+      <c r="F2" s="3" t="n">
+        <v>17.676767</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3">
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>17.11.2025 08:30</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>e62ed41</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>alpha beta pruning</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>108.062364</v>
       </c>
-      <c r="E3" s="3">
-        <v>216.79706678625141</v>
-      </c>
-      <c r="F3" s="3">
-        <v>19.865320000000001</v>
+      <c r="E3" s="3" t="n">
+        <v>216.7970667862514</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>19.86532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3">
-        <v>111.00519300000001</v>
-      </c>
-      <c r="E4" s="3">
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>18.11.2025 16:27</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>32be42e</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>piece square evaluation</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>111.005193</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <v>25066.89199259596</v>
       </c>
-      <c r="F4" s="3">
-        <v>23.905723999999999</v>
+      <c r="F4" s="3" t="n">
+        <v>23.905724</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>45979.688888888886</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4">
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>45979.68888888889</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>0c1055d</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>fixed eval wrong table orientation</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>104.15</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="4" t="n">
         <v>24272.69</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4" t="n">
         <v>28.45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>45979.706250000003</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4">
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>45979.70625</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>ecf1de6</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>iterative deepening</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>107.01</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="4" t="n">
         <v>24990.92</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4" t="n">
         <v>29.8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>18.11.2025 20:12</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Uncommitted changes</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>110.074491</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>19882.5469275052</v>
+      </c>
+      <c r="F7" s="3" t="n">
+        <v>27.609426</v>
       </c>
     </row>
   </sheetData>
@@ -693,6 +755,26 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="colorScale" priority="20">
@@ -715,6 +797,26 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="colorScale" priority="3">
@@ -827,8 +929,28 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00F8696B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="0063BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00F8696B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="0063BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
increased tt size to 4GB
</commit_message>
<xml_diff>
--- a/progress_tracking/progress.xlsx
+++ b/progress_tracking/progress.xlsx
@@ -1,133 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\RustroverProjects\ChessEngine\progress_tracking\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEF9323-FEF8-4F7B-A92C-239646B41B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Progress" sheetId="1" r:id="rId1"/>
+    <sheet name="Progress" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
-  <si>
-    <t>TIMESTAMP</t>
-  </si>
-  <si>
-    <t>COMMIT</t>
-  </si>
-  <si>
-    <t>MESSAGE</t>
-  </si>
-  <si>
-    <t>PERFT (ms)</t>
-  </si>
-  <si>
-    <t>EVAL (ps)</t>
-  </si>
-  <si>
-    <t>SUITE (%)</t>
-  </si>
-  <si>
-    <t>15.11.2025 18:44</t>
-  </si>
-  <si>
-    <t>96ea7fd</t>
-  </si>
-  <si>
-    <t>fixed progress tracking</t>
-  </si>
-  <si>
-    <t>17.11.2025 08:30</t>
-  </si>
-  <si>
-    <t>e62ed41</t>
-  </si>
-  <si>
-    <t>alpha beta pruning</t>
-  </si>
-  <si>
-    <t>18.11.2025 16:27</t>
-  </si>
-  <si>
-    <t>32be42e</t>
-  </si>
-  <si>
-    <t>piece square evaluation</t>
-  </si>
-  <si>
-    <t>0c1055d</t>
-  </si>
-  <si>
-    <t>fixed eval wrong table orientation</t>
-  </si>
-  <si>
-    <t>ecf1de6</t>
-  </si>
-  <si>
-    <t>iterative deepening</t>
-  </si>
-  <si>
-    <t>18.11.2025 20:35</t>
-  </si>
-  <si>
-    <t>b693236</t>
-  </si>
-  <si>
-    <t>integrated material eval into psqt</t>
-  </si>
-  <si>
-    <t>19.11.2025 10:38</t>
-  </si>
-  <si>
-    <t>42816a6</t>
-  </si>
-  <si>
-    <t>implemented transposition table</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Consolas"/>
+      <b val="1"/>
       <sz val="11"/>
-      <name val="Consolas"/>
     </font>
     <font>
+      <name val="Consolas"/>
       <sz val="11"/>
-      <name val="Consolas"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -146,37 +61,96 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -464,179 +438,261 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="20" style="8" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="6" width="14" customWidth="1"/>
+    <col width="20" customWidth="1" style="8" min="1" max="1"/>
+    <col width="12" customWidth="1" min="2" max="2"/>
+    <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="6"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>TIMESTAMP</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>COMMIT</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>MESSAGE</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>PERFT (ms)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>EVAL (ps)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SUITE (%)</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="3">
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>15.11.2025 18:44</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>96ea7fd</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>fixed progress tracking</t>
+        </is>
+      </c>
+      <c r="D2" s="3" t="n">
         <v>104.547059</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="3" t="n">
         <v>208.1159881736437</v>
       </c>
-      <c r="F2" s="3">
-        <v>17.676767000000002</v>
+      <c r="F2" s="3" t="n">
+        <v>17.676767</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="3">
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>17.11.2025 08:30</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>e62ed41</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>alpha beta pruning</t>
+        </is>
+      </c>
+      <c r="D3" s="3" t="n">
         <v>108.062364</v>
       </c>
-      <c r="E3" s="3">
-        <v>216.79706678625141</v>
-      </c>
-      <c r="F3" s="3">
-        <v>19.865320000000001</v>
+      <c r="E3" s="3" t="n">
+        <v>216.7970667862514</v>
+      </c>
+      <c r="F3" s="3" t="n">
+        <v>19.86532</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" s="3">
-        <v>111.00519300000001</v>
-      </c>
-      <c r="E4" s="3">
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>18.11.2025 16:27</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>32be42e</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>piece square evaluation</t>
+        </is>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>111.005193</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <v>25066.89199259596</v>
       </c>
-      <c r="F4" s="3">
-        <v>23.905723999999999</v>
+      <c r="F4" s="3" t="n">
+        <v>23.905724</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
-        <v>45979.688888888893</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="4">
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>45979.68888888889</v>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>0c1055d</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>fixed eval wrong table orientation</t>
+        </is>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>104.15</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="4" t="n">
         <v>24272.69</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="4" t="n">
         <v>28.45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>45979.706250000003</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4">
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>45979.70625</v>
+      </c>
+      <c r="B6" s="4" t="inlineStr">
+        <is>
+          <t>ecf1de6</t>
+        </is>
+      </c>
+      <c r="C6" s="4" t="inlineStr">
+        <is>
+          <t>iterative deepening</t>
+        </is>
+      </c>
+      <c r="D6" s="4" t="n">
         <v>107.01</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="4" t="n">
         <v>24990.92</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="4" t="n">
         <v>29.8</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="3">
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>18.11.2025 20:35</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>b693236</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>integrated material eval into psqt</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="n">
         <v>107.759418</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="3" t="n">
         <v>19513.88065940564</v>
       </c>
-      <c r="F7" s="3">
-        <v>29.292929000000001</v>
+      <c r="F7" s="3" t="n">
+        <v>29.292929</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3">
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>19.11.2025 10:38</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>42816a6</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>implemented transposition table</t>
+        </is>
+      </c>
+      <c r="D8" s="3" t="n">
         <v>128.263248</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="3" t="n">
         <v>19460.41024803367</v>
       </c>
-      <c r="F8" s="3">
-        <v>30.976430000000001</v>
+      <c r="F8" s="3" t="n">
+        <v>30.97643</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>19.11.2025 11:04</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>local</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Uncommitted changes</t>
+        </is>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>132.7052</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>19398.87404920046</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>31.144781</v>
       </c>
     </row>
   </sheetData>
@@ -751,6 +807,16 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="colorScale" priority="20">
@@ -773,6 +839,16 @@
         <color rgb="FFF8696B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="0063BE7B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="00F8696B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="colorScale" priority="3">
@@ -885,8 +961,18 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00F8696B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="0063BE7B"/>
+      </colorScale>
+    </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup orientation="portrait" paperSize="9"/>
 </worksheet>
 </file>
</xml_diff>